<commit_message>
finish eudl to bb activity
</commit_message>
<xml_diff>
--- a/data/reporting/end_user_to_bb_job_role_activity.xlsx
+++ b/data/reporting/end_user_to_bb_job_role_activity.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Role Mapping Report" sheetId="1" r:id="rId1"/>
+    <sheet name="EUDL to Backbone Activities " sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -15,14 +15,14 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Role Mapping Report'!$A$4:$BE$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EUDL to Backbone Activities '!$A$3:$BE$3</definedName>
     <definedName name="Directors">[1]Definitions!$B$75:$C$96</definedName>
     <definedName name="HML">[2]Data!$B$2:$B$4</definedName>
     <definedName name="Org">[2]Data!$C$2:$C$22</definedName>
     <definedName name="Type">[3]Data!$A$1:$A$4</definedName>
     <definedName name="YN">[2]Data!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -417,7 +417,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -441,27 +441,18 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1161,34 +1152,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF4"/>
+  <dimension ref="A1:BF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="22" ySplit="4" topLeftCell="BF5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <pane xSplit="22" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="W1" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="26" defaultRowHeight="15.75" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="8"/>
-    <col min="3" max="7" width="9.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="9.140625" style="8" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="8"/>
-    <col min="10" max="13" width="9.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="9.140625" style="8" collapsed="1"/>
-    <col min="15" max="17" width="9.140625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="19" max="20" width="9.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="9.140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.140625" style="8" customWidth="1"/>
-    <col min="23" max="57" width="9.140625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="9.140625" style="8" collapsed="1"/>
-    <col min="59" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="2" width="7.5703125" style="8" customWidth="1"/>
+    <col min="3" max="7" width="7.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="7.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.5703125" style="8" customWidth="1"/>
+    <col min="10" max="13" width="7.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="7.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="7.5703125" style="8" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="19" max="20" width="7.5703125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="22" width="7.5703125" style="8" customWidth="1"/>
+    <col min="23" max="57" width="7.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="27" style="8" customWidth="1" collapsed="1"/>
+    <col min="59" max="16384" width="26" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="10" customFormat="1" ht="6" customHeight="1">
+    <row r="1" spans="1:57" s="9" customFormat="1" ht="6" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1208,302 +1198,242 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:57" s="16" customFormat="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="15"/>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="15"/>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-      <c r="BB2" s="15"/>
-      <c r="BC2" s="15"/>
-      <c r="BD2" s="15"/>
-      <c r="BE2" s="15"/>
+    <row r="2" spans="1:57" s="10" customFormat="1" ht="162.75" customHeight="1" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AZ2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BD2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE2" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="3" spans="1:57" s="9" customFormat="1" ht="162.75" customHeight="1" thickBot="1">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="V3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="W3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="X3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD3" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM3" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP3" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AQ3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AT3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AU3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="AV3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="AW3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AY3" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AZ3" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="BC3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BD3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE3" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:57" s="2" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7"/>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
-      <c r="AL4" s="7"/>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="7"/>
-      <c r="AU4" s="7"/>
-      <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="7"/>
-      <c r="AY4" s="7"/>
-      <c r="AZ4" s="7"/>
-      <c r="BA4" s="7"/>
-      <c r="BB4" s="7"/>
-      <c r="BC4" s="7"/>
-      <c r="BD4" s="7"/>
-      <c r="BE4" s="7"/>
+    <row r="3" spans="1:57" s="2" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7"/>
+      <c r="AL3" s="7"/>
+      <c r="AM3" s="7"/>
+      <c r="AN3" s="7"/>
+      <c r="AO3" s="7"/>
+      <c r="AP3" s="7"/>
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="7"/>
+      <c r="AT3" s="7"/>
+      <c r="AU3" s="7"/>
+      <c r="AV3" s="7"/>
+      <c r="AW3" s="7"/>
+      <c r="AX3" s="7"/>
+      <c r="AY3" s="7"/>
+      <c r="AZ3" s="7"/>
+      <c r="BA3" s="7"/>
+      <c r="BB3" s="7"/>
+      <c r="BC3" s="7"/>
+      <c r="BD3" s="7"/>
+      <c r="BE3" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:BE4"/>
-  <mergeCells count="2">
+  <autoFilter ref="A3:BE3"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:BE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>

</xml_diff>